<commit_message>
Add UC-18gsm-250W-BFQR film inspection form
- Add HTML form interface for UC-18gsm-250W-BFQR product inspection
- Add JavaScript functionality for form interactions and data handling
- Add Excel template for report generation
- Add backend export functionality for UC-18gsm-250W-BFQR forms
</commit_message>
<xml_diff>
--- a/backend/templates/UC-18gsm-250W-BFQR.xlsx
+++ b/backend/templates/UC-18gsm-250W-BFQR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7A8DDD-0A45-408B-9D66-FB277C989CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E870AAB6-61A0-4D02-B52E-3F81CFDE7565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="6" r:id="rId1"/>
@@ -28,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -2007,6 +2010,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2056,6 +2065,12 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2391,18 +2406,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3925,7 +3928,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I7" sqref="I7:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4014,11 +4017,11 @@
       <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="304">
+      <c r="J4" s="178">
         <f>Page1!J4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="305"/>
+      <c r="K4" s="179"/>
     </row>
     <row r="5" spans="1:11" s="45" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="147" t="s">
@@ -4050,104 +4053,104 @@
       <c r="I5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="306">
+      <c r="J5" s="194">
         <f>Page1!J5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="307"/>
+      <c r="K5" s="195"/>
     </row>
     <row r="6" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="208" t="s">
+      <c r="A6" s="212" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="209"/>
-      <c r="C6" s="210"/>
-      <c r="D6" s="192"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="183"/>
-      <c r="G6" s="182"/>
-      <c r="H6" s="183"/>
-      <c r="I6" s="206"/>
-      <c r="J6" s="207"/>
+      <c r="B6" s="213"/>
+      <c r="C6" s="214"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="184"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="210"/>
+      <c r="J6" s="211"/>
       <c r="K6" s="55"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="192" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="193"/>
-      <c r="C7" s="193"/>
-      <c r="D7" s="211" t="s">
+      <c r="A7" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="197"/>
+      <c r="C7" s="197"/>
+      <c r="D7" s="215" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="193"/>
+      <c r="E7" s="197"/>
       <c r="F7" s="177"/>
-      <c r="G7" s="182" t="s">
+      <c r="G7" s="184" t="s">
         <v>125</v>
       </c>
-      <c r="H7" s="193"/>
-      <c r="I7" s="182" t="s">
+      <c r="H7" s="197"/>
+      <c r="I7" s="184" t="s">
         <v>135</v>
       </c>
-      <c r="J7" s="183"/>
-      <c r="K7" s="199" t="s">
+      <c r="J7" s="185"/>
+      <c r="K7" s="203" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="194"/>
-      <c r="B8" s="195"/>
-      <c r="C8" s="195"/>
-      <c r="D8" s="194" t="s">
+      <c r="A8" s="198"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="203" t="s">
+      <c r="E8" s="207" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="204" t="s">
+      <c r="F8" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="196"/>
-      <c r="H8" s="195"/>
-      <c r="I8" s="196" t="s">
+      <c r="G8" s="200"/>
+      <c r="H8" s="199"/>
+      <c r="I8" s="200" t="s">
         <v>136</v>
       </c>
-      <c r="J8" s="204"/>
-      <c r="K8" s="200"/>
+      <c r="J8" s="208"/>
+      <c r="K8" s="204"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="194"/>
-      <c r="B9" s="195"/>
-      <c r="C9" s="195"/>
-      <c r="D9" s="194"/>
+      <c r="A9" s="198"/>
+      <c r="B9" s="199"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="198"/>
       <c r="E9" s="151"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="195"/>
+      <c r="F9" s="208"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="199"/>
       <c r="I9" s="57" t="s">
         <v>123</v>
       </c>
       <c r="J9" s="58">
-        <v>210</v>
-      </c>
-      <c r="K9" s="200"/>
+        <v>250</v>
+      </c>
+      <c r="K9" s="204"/>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="194"/>
-      <c r="B10" s="195"/>
-      <c r="C10" s="195"/>
-      <c r="D10" s="202"/>
+      <c r="A10" s="198"/>
+      <c r="B10" s="199"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="206"/>
       <c r="E10" s="152"/>
-      <c r="F10" s="205"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="198"/>
+      <c r="F10" s="209"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="202"/>
       <c r="I10" s="59" t="s">
         <v>124</v>
       </c>
       <c r="J10" s="60">
-        <v>213</v>
-      </c>
-      <c r="K10" s="201"/>
+        <v>253</v>
+      </c>
+      <c r="K10" s="205"/>
     </row>
     <row r="11" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="120">
@@ -4165,10 +4168,10 @@
       <c r="D11" s="61"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
-      <c r="G11" s="191"/>
-      <c r="H11" s="191"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="179"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="193"/>
+      <c r="I11" s="180"/>
+      <c r="J11" s="181"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4187,10 +4190,10 @@
       <c r="D12" s="63"/>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
-      <c r="G12" s="190"/>
-      <c r="H12" s="190"/>
-      <c r="I12" s="180"/>
-      <c r="J12" s="181"/>
+      <c r="G12" s="192"/>
+      <c r="H12" s="192"/>
+      <c r="I12" s="182"/>
+      <c r="J12" s="183"/>
       <c r="K12" s="64"/>
     </row>
     <row r="13" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4209,10 +4212,10 @@
       <c r="D13" s="63"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="190"/>
-      <c r="H13" s="190"/>
-      <c r="I13" s="180"/>
-      <c r="J13" s="181"/>
+      <c r="G13" s="192"/>
+      <c r="H13" s="192"/>
+      <c r="I13" s="182"/>
+      <c r="J13" s="183"/>
       <c r="K13" s="64"/>
     </row>
     <row r="14" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4231,10 +4234,10 @@
       <c r="D14" s="63"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="190"/>
-      <c r="H14" s="190"/>
-      <c r="I14" s="180"/>
-      <c r="J14" s="181"/>
+      <c r="G14" s="192"/>
+      <c r="H14" s="192"/>
+      <c r="I14" s="182"/>
+      <c r="J14" s="183"/>
       <c r="K14" s="64"/>
     </row>
     <row r="15" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4253,10 +4256,10 @@
       <c r="D15" s="63"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="190"/>
-      <c r="H15" s="190"/>
-      <c r="I15" s="180"/>
-      <c r="J15" s="181"/>
+      <c r="G15" s="192"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="182"/>
+      <c r="J15" s="183"/>
       <c r="K15" s="64"/>
     </row>
     <row r="16" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4275,10 +4278,10 @@
       <c r="D16" s="61"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="191"/>
-      <c r="H16" s="191"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="181"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="182"/>
+      <c r="J16" s="183"/>
       <c r="K16" s="62"/>
     </row>
     <row r="17" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4297,10 +4300,10 @@
       <c r="D17" s="63"/>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
-      <c r="G17" s="190"/>
-      <c r="H17" s="190"/>
-      <c r="I17" s="180"/>
-      <c r="J17" s="181"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="183"/>
       <c r="K17" s="64"/>
     </row>
     <row r="18" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4319,10 +4322,10 @@
       <c r="D18" s="63"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
-      <c r="G18" s="190"/>
-      <c r="H18" s="190"/>
-      <c r="I18" s="180"/>
-      <c r="J18" s="181"/>
+      <c r="G18" s="192"/>
+      <c r="H18" s="192"/>
+      <c r="I18" s="182"/>
+      <c r="J18" s="183"/>
       <c r="K18" s="64"/>
     </row>
     <row r="19" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4341,10 +4344,10 @@
       <c r="D19" s="63"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="190"/>
-      <c r="H19" s="190"/>
-      <c r="I19" s="180"/>
-      <c r="J19" s="181"/>
+      <c r="G19" s="192"/>
+      <c r="H19" s="192"/>
+      <c r="I19" s="182"/>
+      <c r="J19" s="183"/>
       <c r="K19" s="64"/>
     </row>
     <row r="20" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4363,10 +4366,10 @@
       <c r="D20" s="63"/>
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="186"/>
-      <c r="H20" s="187"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="181"/>
+      <c r="G20" s="188"/>
+      <c r="H20" s="189"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="183"/>
       <c r="K20" s="64"/>
     </row>
     <row r="21" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4385,10 +4388,10 @@
       <c r="D21" s="63"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
-      <c r="G21" s="186"/>
-      <c r="H21" s="187"/>
-      <c r="I21" s="180"/>
-      <c r="J21" s="181"/>
+      <c r="G21" s="188"/>
+      <c r="H21" s="189"/>
+      <c r="I21" s="182"/>
+      <c r="J21" s="183"/>
       <c r="K21" s="64"/>
     </row>
     <row r="22" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4407,10 +4410,10 @@
       <c r="D22" s="63"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
-      <c r="G22" s="186"/>
-      <c r="H22" s="187"/>
-      <c r="I22" s="180"/>
-      <c r="J22" s="181"/>
+      <c r="G22" s="188"/>
+      <c r="H22" s="189"/>
+      <c r="I22" s="182"/>
+      <c r="J22" s="183"/>
       <c r="K22" s="64"/>
     </row>
     <row r="23" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4429,10 +4432,10 @@
       <c r="D23" s="63"/>
       <c r="E23" s="25"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="186"/>
-      <c r="H23" s="187"/>
-      <c r="I23" s="180"/>
-      <c r="J23" s="181"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="189"/>
+      <c r="I23" s="182"/>
+      <c r="J23" s="183"/>
       <c r="K23" s="64"/>
     </row>
     <row r="24" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4451,10 +4454,10 @@
       <c r="D24" s="63"/>
       <c r="E24" s="25"/>
       <c r="F24" s="25"/>
-      <c r="G24" s="186"/>
-      <c r="H24" s="187"/>
-      <c r="I24" s="180"/>
-      <c r="J24" s="181"/>
+      <c r="G24" s="188"/>
+      <c r="H24" s="189"/>
+      <c r="I24" s="182"/>
+      <c r="J24" s="183"/>
       <c r="K24" s="64"/>
     </row>
     <row r="25" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4473,10 +4476,10 @@
       <c r="D25" s="63"/>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="186"/>
-      <c r="H25" s="187"/>
-      <c r="I25" s="180"/>
-      <c r="J25" s="181"/>
+      <c r="G25" s="188"/>
+      <c r="H25" s="189"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="183"/>
       <c r="K25" s="64"/>
     </row>
     <row r="26" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4495,10 +4498,10 @@
       <c r="D26" s="63"/>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
-      <c r="G26" s="186"/>
-      <c r="H26" s="187"/>
-      <c r="I26" s="180"/>
-      <c r="J26" s="181"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="189"/>
+      <c r="I26" s="182"/>
+      <c r="J26" s="183"/>
       <c r="K26" s="64"/>
     </row>
     <row r="27" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4517,10 +4520,10 @@
       <c r="D27" s="63"/>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
-      <c r="G27" s="186"/>
-      <c r="H27" s="187"/>
-      <c r="I27" s="180"/>
-      <c r="J27" s="181"/>
+      <c r="G27" s="188"/>
+      <c r="H27" s="189"/>
+      <c r="I27" s="182"/>
+      <c r="J27" s="183"/>
       <c r="K27" s="64"/>
     </row>
     <row r="28" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4539,10 +4542,10 @@
       <c r="D28" s="63"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
-      <c r="G28" s="186"/>
-      <c r="H28" s="187"/>
-      <c r="I28" s="180"/>
-      <c r="J28" s="181"/>
+      <c r="G28" s="188"/>
+      <c r="H28" s="189"/>
+      <c r="I28" s="182"/>
+      <c r="J28" s="183"/>
       <c r="K28" s="64"/>
     </row>
     <row r="29" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4561,10 +4564,10 @@
       <c r="D29" s="63"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="186"/>
-      <c r="H29" s="187"/>
-      <c r="I29" s="180"/>
-      <c r="J29" s="181"/>
+      <c r="G29" s="188"/>
+      <c r="H29" s="189"/>
+      <c r="I29" s="182"/>
+      <c r="J29" s="183"/>
       <c r="K29" s="64"/>
     </row>
     <row r="30" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4583,10 +4586,10 @@
       <c r="D30" s="63"/>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
-      <c r="G30" s="186"/>
-      <c r="H30" s="187"/>
-      <c r="I30" s="180"/>
-      <c r="J30" s="181"/>
+      <c r="G30" s="188"/>
+      <c r="H30" s="189"/>
+      <c r="I30" s="182"/>
+      <c r="J30" s="183"/>
       <c r="K30" s="64"/>
     </row>
     <row r="31" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4605,10 +4608,10 @@
       <c r="D31" s="63"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
-      <c r="G31" s="186"/>
-      <c r="H31" s="187"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="181"/>
+      <c r="G31" s="188"/>
+      <c r="H31" s="189"/>
+      <c r="I31" s="182"/>
+      <c r="J31" s="183"/>
       <c r="K31" s="64"/>
     </row>
     <row r="32" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4627,10 +4630,10 @@
       <c r="D32" s="63"/>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
-      <c r="G32" s="186"/>
-      <c r="H32" s="187"/>
-      <c r="I32" s="180"/>
-      <c r="J32" s="181"/>
+      <c r="G32" s="188"/>
+      <c r="H32" s="189"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="183"/>
       <c r="K32" s="64"/>
     </row>
     <row r="33" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4649,10 +4652,10 @@
       <c r="D33" s="63"/>
       <c r="E33" s="25"/>
       <c r="F33" s="25"/>
-      <c r="G33" s="186"/>
-      <c r="H33" s="187"/>
-      <c r="I33" s="180"/>
-      <c r="J33" s="181"/>
+      <c r="G33" s="188"/>
+      <c r="H33" s="189"/>
+      <c r="I33" s="182"/>
+      <c r="J33" s="183"/>
       <c r="K33" s="64"/>
     </row>
     <row r="34" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4671,10 +4674,10 @@
       <c r="D34" s="63"/>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
-      <c r="G34" s="186"/>
-      <c r="H34" s="187"/>
-      <c r="I34" s="180"/>
-      <c r="J34" s="181"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="189"/>
+      <c r="I34" s="182"/>
+      <c r="J34" s="183"/>
       <c r="K34" s="64"/>
     </row>
     <row r="35" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4693,10 +4696,10 @@
       <c r="D35" s="63"/>
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
-      <c r="G35" s="186"/>
-      <c r="H35" s="187"/>
-      <c r="I35" s="180"/>
-      <c r="J35" s="181"/>
+      <c r="G35" s="188"/>
+      <c r="H35" s="189"/>
+      <c r="I35" s="182"/>
+      <c r="J35" s="183"/>
       <c r="K35" s="64"/>
     </row>
     <row r="36" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4715,10 +4718,10 @@
       <c r="D36" s="63"/>
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
-      <c r="G36" s="186"/>
-      <c r="H36" s="187"/>
-      <c r="I36" s="180"/>
-      <c r="J36" s="181"/>
+      <c r="G36" s="188"/>
+      <c r="H36" s="189"/>
+      <c r="I36" s="182"/>
+      <c r="J36" s="183"/>
       <c r="K36" s="64"/>
     </row>
     <row r="37" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4737,10 +4740,10 @@
       <c r="D37" s="63"/>
       <c r="E37" s="25"/>
       <c r="F37" s="25"/>
-      <c r="G37" s="186"/>
-      <c r="H37" s="187"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="181"/>
+      <c r="G37" s="188"/>
+      <c r="H37" s="189"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="183"/>
       <c r="K37" s="64"/>
     </row>
     <row r="38" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4759,10 +4762,10 @@
       <c r="D38" s="63"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
-      <c r="G38" s="186"/>
-      <c r="H38" s="187"/>
-      <c r="I38" s="180"/>
-      <c r="J38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="189"/>
+      <c r="I38" s="182"/>
+      <c r="J38" s="183"/>
       <c r="K38" s="64"/>
     </row>
     <row r="39" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4781,10 +4784,10 @@
       <c r="D39" s="63"/>
       <c r="E39" s="25"/>
       <c r="F39" s="25"/>
-      <c r="G39" s="186"/>
-      <c r="H39" s="187"/>
-      <c r="I39" s="180"/>
-      <c r="J39" s="181"/>
+      <c r="G39" s="188"/>
+      <c r="H39" s="189"/>
+      <c r="I39" s="182"/>
+      <c r="J39" s="183"/>
       <c r="K39" s="64"/>
     </row>
     <row r="40" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4803,10 +4806,10 @@
       <c r="D40" s="63"/>
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
-      <c r="G40" s="190"/>
-      <c r="H40" s="190"/>
-      <c r="I40" s="180"/>
-      <c r="J40" s="181"/>
+      <c r="G40" s="192"/>
+      <c r="H40" s="192"/>
+      <c r="I40" s="182"/>
+      <c r="J40" s="183"/>
       <c r="K40" s="64"/>
     </row>
     <row r="41" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4827,16 +4830,16 @@
         <f>AVERAGE(F11:F40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G41" s="188" t="e">
+      <c r="G41" s="190" t="e">
         <f>AVERAGE(G11:H40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="189"/>
-      <c r="I41" s="220" t="e">
+      <c r="H41" s="191"/>
+      <c r="I41" s="224" t="e">
         <f>AVERAGE(I11:J40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J41" s="221"/>
+      <c r="J41" s="225"/>
       <c r="K41" s="37" t="e">
         <f>AVERAGE(K11:K40)</f>
         <v>#DIV/0!</v>
@@ -4860,27 +4863,27 @@
         <f>MIN(F11:F40)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="184">
+      <c r="G42" s="186">
         <f>MIN(G11:H40)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="185"/>
-      <c r="I42" s="218">
+      <c r="H42" s="187"/>
+      <c r="I42" s="222">
         <f>MIN(I11:J40)</f>
         <v>0</v>
       </c>
-      <c r="J42" s="219"/>
+      <c r="J42" s="223"/>
       <c r="K42" s="40">
         <f>MIN(K11:K40)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="216" t="s">
+      <c r="A43" s="220" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="217"/>
-      <c r="C43" s="217"/>
+      <c r="B43" s="221"/>
+      <c r="C43" s="221"/>
       <c r="D43" s="67">
         <f>MAX(D11:D40)</f>
         <v>0</v>
@@ -4893,16 +4896,16 @@
         <f>MAX(F11:F40)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="212">
+      <c r="G43" s="216">
         <f>MAX(G11:H40)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="213"/>
-      <c r="I43" s="214">
+      <c r="H43" s="217"/>
+      <c r="I43" s="218">
         <f>MAX(I11:J40)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="215"/>
+      <c r="J43" s="219"/>
       <c r="K43" s="69">
         <f>MAX(K11:K40)</f>
         <v>0</v>
@@ -5248,11 +5251,11 @@
       <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="304">
+      <c r="J4" s="178">
         <f>Page1!J4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="305"/>
+      <c r="K4" s="179"/>
     </row>
     <row r="5" spans="1:11" s="45" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="147" t="s">
@@ -5284,79 +5287,79 @@
       <c r="I5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="306">
+      <c r="J5" s="194">
         <f>Page1!J5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="307"/>
+      <c r="K5" s="195"/>
     </row>
     <row r="6" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="225" t="s">
+      <c r="A6" s="229" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="227"/>
-      <c r="D6" s="228"/>
+      <c r="B6" s="230"/>
+      <c r="C6" s="231"/>
+      <c r="D6" s="232"/>
       <c r="E6" s="134"/>
       <c r="F6" s="134"/>
       <c r="G6" s="154"/>
       <c r="H6" s="71"/>
-      <c r="I6" s="192"/>
-      <c r="J6" s="193"/>
-      <c r="K6" s="199"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="203"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="192" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="193"/>
-      <c r="C7" s="193"/>
-      <c r="D7" s="211" t="s">
+      <c r="A7" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="197"/>
+      <c r="C7" s="197"/>
+      <c r="D7" s="215" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229"/>
+      <c r="E7" s="233"/>
+      <c r="F7" s="233"/>
       <c r="G7" s="177"/>
-      <c r="H7" s="222" t="s">
+      <c r="H7" s="226" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="194"/>
-      <c r="J7" s="195"/>
-      <c r="K7" s="200"/>
+      <c r="I7" s="198"/>
+      <c r="J7" s="199"/>
+      <c r="K7" s="204"/>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="194"/>
-      <c r="B8" s="195"/>
-      <c r="C8" s="195"/>
-      <c r="D8" s="232" t="s">
+      <c r="A8" s="198"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="236" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="203" t="s">
+      <c r="E8" s="207" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="203" t="s">
+      <c r="F8" s="207" t="s">
         <v>131</v>
       </c>
-      <c r="G8" s="203" t="s">
+      <c r="G8" s="207" t="s">
         <v>128</v>
       </c>
-      <c r="H8" s="223"/>
-      <c r="I8" s="194"/>
-      <c r="J8" s="195"/>
-      <c r="K8" s="200"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="198"/>
+      <c r="J8" s="199"/>
+      <c r="K8" s="204"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="194"/>
-      <c r="B9" s="195"/>
-      <c r="C9" s="195"/>
-      <c r="D9" s="233"/>
+      <c r="A9" s="198"/>
+      <c r="B9" s="199"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="237"/>
       <c r="E9" s="152"/>
       <c r="F9" s="152"/>
       <c r="G9" s="152"/>
-      <c r="H9" s="224"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="195"/>
-      <c r="K9" s="200"/>
+      <c r="H9" s="228"/>
+      <c r="I9" s="198"/>
+      <c r="J9" s="199"/>
+      <c r="K9" s="204"/>
     </row>
     <row r="10" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="120">
@@ -5376,9 +5379,9 @@
       <c r="F10" s="23"/>
       <c r="G10" s="73"/>
       <c r="H10" s="74"/>
-      <c r="I10" s="194"/>
-      <c r="J10" s="195"/>
-      <c r="K10" s="200"/>
+      <c r="I10" s="198"/>
+      <c r="J10" s="199"/>
+      <c r="K10" s="204"/>
     </row>
     <row r="11" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="123">
@@ -5398,9 +5401,9 @@
       <c r="F11" s="26"/>
       <c r="G11" s="76"/>
       <c r="H11" s="77"/>
-      <c r="I11" s="194"/>
-      <c r="J11" s="195"/>
-      <c r="K11" s="200"/>
+      <c r="I11" s="198"/>
+      <c r="J11" s="199"/>
+      <c r="K11" s="204"/>
     </row>
     <row r="12" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="123">
@@ -5420,9 +5423,9 @@
       <c r="F12" s="26"/>
       <c r="G12" s="76"/>
       <c r="H12" s="77"/>
-      <c r="I12" s="194"/>
-      <c r="J12" s="195"/>
-      <c r="K12" s="200"/>
+      <c r="I12" s="198"/>
+      <c r="J12" s="199"/>
+      <c r="K12" s="204"/>
     </row>
     <row r="13" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="123">
@@ -5442,9 +5445,9 @@
       <c r="F13" s="23"/>
       <c r="G13" s="73"/>
       <c r="H13" s="77"/>
-      <c r="I13" s="194"/>
-      <c r="J13" s="195"/>
-      <c r="K13" s="200"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="199"/>
+      <c r="K13" s="204"/>
     </row>
     <row r="14" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="123">
@@ -5464,9 +5467,9 @@
       <c r="F14" s="26"/>
       <c r="G14" s="76"/>
       <c r="H14" s="77"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="195"/>
-      <c r="K14" s="200"/>
+      <c r="I14" s="198"/>
+      <c r="J14" s="199"/>
+      <c r="K14" s="204"/>
     </row>
     <row r="15" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="123">
@@ -5486,9 +5489,9 @@
       <c r="F15" s="26"/>
       <c r="G15" s="76"/>
       <c r="H15" s="77"/>
-      <c r="I15" s="194"/>
-      <c r="J15" s="195"/>
-      <c r="K15" s="200"/>
+      <c r="I15" s="198"/>
+      <c r="J15" s="199"/>
+      <c r="K15" s="204"/>
     </row>
     <row r="16" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="123">
@@ -5508,9 +5511,9 @@
       <c r="F16" s="26"/>
       <c r="G16" s="76"/>
       <c r="H16" s="77"/>
-      <c r="I16" s="194"/>
-      <c r="J16" s="195"/>
-      <c r="K16" s="200"/>
+      <c r="I16" s="198"/>
+      <c r="J16" s="199"/>
+      <c r="K16" s="204"/>
     </row>
     <row r="17" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="123">
@@ -5530,9 +5533,9 @@
       <c r="F17" s="26"/>
       <c r="G17" s="76"/>
       <c r="H17" s="77"/>
-      <c r="I17" s="194"/>
-      <c r="J17" s="195"/>
-      <c r="K17" s="200"/>
+      <c r="I17" s="198"/>
+      <c r="J17" s="199"/>
+      <c r="K17" s="204"/>
     </row>
     <row r="18" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="123">
@@ -5552,9 +5555,9 @@
       <c r="F18" s="26"/>
       <c r="G18" s="76"/>
       <c r="H18" s="77"/>
-      <c r="I18" s="194"/>
-      <c r="J18" s="195"/>
-      <c r="K18" s="200"/>
+      <c r="I18" s="198"/>
+      <c r="J18" s="199"/>
+      <c r="K18" s="204"/>
     </row>
     <row r="19" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="123">
@@ -5574,9 +5577,9 @@
       <c r="F19" s="26"/>
       <c r="G19" s="76"/>
       <c r="H19" s="77"/>
-      <c r="I19" s="194"/>
-      <c r="J19" s="195"/>
-      <c r="K19" s="200"/>
+      <c r="I19" s="198"/>
+      <c r="J19" s="199"/>
+      <c r="K19" s="204"/>
     </row>
     <row r="20" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="129">
@@ -5596,9 +5599,9 @@
       <c r="F20" s="26"/>
       <c r="G20" s="76"/>
       <c r="H20" s="77"/>
-      <c r="I20" s="194"/>
-      <c r="J20" s="195"/>
-      <c r="K20" s="200"/>
+      <c r="I20" s="198"/>
+      <c r="J20" s="199"/>
+      <c r="K20" s="204"/>
     </row>
     <row r="21" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="123">
@@ -5618,9 +5621,9 @@
       <c r="F21" s="26"/>
       <c r="G21" s="76"/>
       <c r="H21" s="77"/>
-      <c r="I21" s="194"/>
-      <c r="J21" s="195"/>
-      <c r="K21" s="200"/>
+      <c r="I21" s="198"/>
+      <c r="J21" s="199"/>
+      <c r="K21" s="204"/>
     </row>
     <row r="22" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="123">
@@ -5640,9 +5643,9 @@
       <c r="F22" s="26"/>
       <c r="G22" s="76"/>
       <c r="H22" s="77"/>
-      <c r="I22" s="194"/>
-      <c r="J22" s="195"/>
-      <c r="K22" s="200"/>
+      <c r="I22" s="198"/>
+      <c r="J22" s="199"/>
+      <c r="K22" s="204"/>
     </row>
     <row r="23" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="123">
@@ -5662,9 +5665,9 @@
       <c r="F23" s="26"/>
       <c r="G23" s="76"/>
       <c r="H23" s="77"/>
-      <c r="I23" s="194"/>
-      <c r="J23" s="195"/>
-      <c r="K23" s="200"/>
+      <c r="I23" s="198"/>
+      <c r="J23" s="199"/>
+      <c r="K23" s="204"/>
     </row>
     <row r="24" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="123">
@@ -5684,9 +5687,9 @@
       <c r="F24" s="26"/>
       <c r="G24" s="76"/>
       <c r="H24" s="77"/>
-      <c r="I24" s="194"/>
-      <c r="J24" s="195"/>
-      <c r="K24" s="200"/>
+      <c r="I24" s="198"/>
+      <c r="J24" s="199"/>
+      <c r="K24" s="204"/>
     </row>
     <row r="25" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="123">
@@ -5706,9 +5709,9 @@
       <c r="F25" s="26"/>
       <c r="G25" s="76"/>
       <c r="H25" s="77"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="195"/>
-      <c r="K25" s="200"/>
+      <c r="I25" s="198"/>
+      <c r="J25" s="199"/>
+      <c r="K25" s="204"/>
     </row>
     <row r="26" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="123">
@@ -5728,9 +5731,9 @@
       <c r="F26" s="26"/>
       <c r="G26" s="76"/>
       <c r="H26" s="77"/>
-      <c r="I26" s="194"/>
-      <c r="J26" s="195"/>
-      <c r="K26" s="200"/>
+      <c r="I26" s="198"/>
+      <c r="J26" s="199"/>
+      <c r="K26" s="204"/>
     </row>
     <row r="27" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="123">
@@ -5750,9 +5753,9 @@
       <c r="F27" s="26"/>
       <c r="G27" s="76"/>
       <c r="H27" s="77"/>
-      <c r="I27" s="194"/>
-      <c r="J27" s="195"/>
-      <c r="K27" s="200"/>
+      <c r="I27" s="198"/>
+      <c r="J27" s="199"/>
+      <c r="K27" s="204"/>
     </row>
     <row r="28" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="123">
@@ -5772,9 +5775,9 @@
       <c r="F28" s="26"/>
       <c r="G28" s="76"/>
       <c r="H28" s="77"/>
-      <c r="I28" s="194"/>
-      <c r="J28" s="195"/>
-      <c r="K28" s="200"/>
+      <c r="I28" s="198"/>
+      <c r="J28" s="199"/>
+      <c r="K28" s="204"/>
     </row>
     <row r="29" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="123">
@@ -5794,9 +5797,9 @@
       <c r="F29" s="26"/>
       <c r="G29" s="76"/>
       <c r="H29" s="77"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="195"/>
-      <c r="K29" s="200"/>
+      <c r="I29" s="198"/>
+      <c r="J29" s="199"/>
+      <c r="K29" s="204"/>
     </row>
     <row r="30" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="129">
@@ -5816,9 +5819,9 @@
       <c r="F30" s="26"/>
       <c r="G30" s="76"/>
       <c r="H30" s="77"/>
-      <c r="I30" s="194"/>
-      <c r="J30" s="195"/>
-      <c r="K30" s="200"/>
+      <c r="I30" s="198"/>
+      <c r="J30" s="199"/>
+      <c r="K30" s="204"/>
     </row>
     <row r="31" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="123">
@@ -5838,9 +5841,9 @@
       <c r="F31" s="26"/>
       <c r="G31" s="76"/>
       <c r="H31" s="77"/>
-      <c r="I31" s="194"/>
-      <c r="J31" s="195"/>
-      <c r="K31" s="200"/>
+      <c r="I31" s="198"/>
+      <c r="J31" s="199"/>
+      <c r="K31" s="204"/>
     </row>
     <row r="32" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="123">
@@ -5860,9 +5863,9 @@
       <c r="F32" s="26"/>
       <c r="G32" s="76"/>
       <c r="H32" s="77"/>
-      <c r="I32" s="194"/>
-      <c r="J32" s="195"/>
-      <c r="K32" s="200"/>
+      <c r="I32" s="198"/>
+      <c r="J32" s="199"/>
+      <c r="K32" s="204"/>
     </row>
     <row r="33" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="123">
@@ -5882,9 +5885,9 @@
       <c r="F33" s="26"/>
       <c r="G33" s="76"/>
       <c r="H33" s="77"/>
-      <c r="I33" s="194"/>
-      <c r="J33" s="195"/>
-      <c r="K33" s="200"/>
+      <c r="I33" s="198"/>
+      <c r="J33" s="199"/>
+      <c r="K33" s="204"/>
     </row>
     <row r="34" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="123">
@@ -5904,9 +5907,9 @@
       <c r="F34" s="26"/>
       <c r="G34" s="76"/>
       <c r="H34" s="77"/>
-      <c r="I34" s="194"/>
-      <c r="J34" s="195"/>
-      <c r="K34" s="200"/>
+      <c r="I34" s="198"/>
+      <c r="J34" s="199"/>
+      <c r="K34" s="204"/>
     </row>
     <row r="35" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="123">
@@ -5926,9 +5929,9 @@
       <c r="F35" s="26"/>
       <c r="G35" s="76"/>
       <c r="H35" s="77"/>
-      <c r="I35" s="194"/>
-      <c r="J35" s="195"/>
-      <c r="K35" s="200"/>
+      <c r="I35" s="198"/>
+      <c r="J35" s="199"/>
+      <c r="K35" s="204"/>
     </row>
     <row r="36" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="123">
@@ -5948,9 +5951,9 @@
       <c r="F36" s="26"/>
       <c r="G36" s="76"/>
       <c r="H36" s="77"/>
-      <c r="I36" s="194"/>
-      <c r="J36" s="195"/>
-      <c r="K36" s="200"/>
+      <c r="I36" s="198"/>
+      <c r="J36" s="199"/>
+      <c r="K36" s="204"/>
     </row>
     <row r="37" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="123">
@@ -5970,9 +5973,9 @@
       <c r="F37" s="26"/>
       <c r="G37" s="76"/>
       <c r="H37" s="77"/>
-      <c r="I37" s="194"/>
-      <c r="J37" s="195"/>
-      <c r="K37" s="200"/>
+      <c r="I37" s="198"/>
+      <c r="J37" s="199"/>
+      <c r="K37" s="204"/>
     </row>
     <row r="38" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="123">
@@ -5992,9 +5995,9 @@
       <c r="F38" s="26"/>
       <c r="G38" s="76"/>
       <c r="H38" s="77"/>
-      <c r="I38" s="194"/>
-      <c r="J38" s="195"/>
-      <c r="K38" s="200"/>
+      <c r="I38" s="198"/>
+      <c r="J38" s="199"/>
+      <c r="K38" s="204"/>
     </row>
     <row r="39" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="130">
@@ -6014,16 +6017,16 @@
       <c r="F39" s="26"/>
       <c r="G39" s="76"/>
       <c r="H39" s="77"/>
-      <c r="I39" s="194"/>
-      <c r="J39" s="195"/>
-      <c r="K39" s="200"/>
+      <c r="I39" s="198"/>
+      <c r="J39" s="199"/>
+      <c r="K39" s="204"/>
     </row>
     <row r="40" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="230" t="s">
+      <c r="A40" s="234" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="231"/>
-      <c r="C40" s="231"/>
+      <c r="B40" s="235"/>
+      <c r="C40" s="235"/>
       <c r="D40" s="78" t="e">
         <f>AVERAGE(D10:D39)</f>
         <v>#DIV/0!</v>
@@ -6044,9 +6047,9 @@
         <f>AVERAGE(H10:H39)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="195"/>
-      <c r="J40" s="195"/>
-      <c r="K40" s="200"/>
+      <c r="I40" s="199"/>
+      <c r="J40" s="199"/>
+      <c r="K40" s="204"/>
     </row>
     <row r="41" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="174" t="s">
@@ -6074,16 +6077,16 @@
         <f>MIN(H10:H39)</f>
         <v>0</v>
       </c>
-      <c r="I41" s="195"/>
-      <c r="J41" s="195"/>
-      <c r="K41" s="200"/>
+      <c r="I41" s="199"/>
+      <c r="J41" s="199"/>
+      <c r="K41" s="204"/>
     </row>
     <row r="42" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="216" t="s">
+      <c r="A42" s="220" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="217"/>
-      <c r="C42" s="217"/>
+      <c r="B42" s="221"/>
+      <c r="C42" s="221"/>
       <c r="D42" s="82">
         <f>MAX(D10:D39)</f>
         <v>0</v>
@@ -6104,9 +6107,9 @@
         <f>MAX(H10:H39)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="198"/>
-      <c r="J42" s="198"/>
-      <c r="K42" s="201"/>
+      <c r="I42" s="202"/>
+      <c r="J42" s="202"/>
+      <c r="K42" s="205"/>
     </row>
     <row r="43" spans="1:11" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
@@ -6262,15 +6265,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="288" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="285"/>
-      <c r="C1" s="285"/>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="286"/>
+      <c r="B1" s="289"/>
+      <c r="C1" s="289"/>
+      <c r="D1" s="289"/>
+      <c r="E1" s="289"/>
+      <c r="F1" s="289"/>
+      <c r="G1" s="290"/>
     </row>
     <row r="2" spans="1:7" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="87"/>
@@ -6284,37 +6287,37 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="86" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="292" t="s">
+      <c r="A3" s="296" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="293"/>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="294"/>
+      <c r="B3" s="297"/>
+      <c r="C3" s="297"/>
+      <c r="D3" s="297"/>
+      <c r="E3" s="297"/>
+      <c r="F3" s="297"/>
+      <c r="G3" s="298"/>
     </row>
     <row r="4" spans="1:7" s="86" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="194" t="s">
+      <c r="A4" s="198" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="195"/>
-      <c r="C4" s="195"/>
-      <c r="D4" s="195"/>
-      <c r="E4" s="195"/>
-      <c r="F4" s="195"/>
-      <c r="G4" s="200"/>
+      <c r="B4" s="199"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="199"/>
+      <c r="G4" s="204"/>
     </row>
     <row r="5" spans="1:7" s="86" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="287" t="s">
+      <c r="A5" s="291" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="288"/>
-      <c r="C5" s="288"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="288"/>
-      <c r="F5" s="288"/>
-      <c r="G5" s="289"/>
+      <c r="B5" s="292"/>
+      <c r="C5" s="292"/>
+      <c r="D5" s="292"/>
+      <c r="E5" s="292"/>
+      <c r="F5" s="292"/>
+      <c r="G5" s="293"/>
     </row>
     <row r="6" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="90" t="s">
@@ -6326,14 +6329,14 @@
       <c r="C6" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="252" t="s">
+      <c r="D6" s="256" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="254"/>
-      <c r="F6" s="290" t="s">
+      <c r="E6" s="258"/>
+      <c r="F6" s="294" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="275">
+      <c r="G6" s="279">
         <f>Page1!J4</f>
         <v>0</v>
       </c>
@@ -6346,13 +6349,13 @@
       <c r="C7" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="252">
+      <c r="D7" s="256">
         <f>Page1!F5</f>
         <v>0</v>
       </c>
-      <c r="E7" s="254"/>
-      <c r="F7" s="290"/>
-      <c r="G7" s="291"/>
+      <c r="E7" s="258"/>
+      <c r="F7" s="294"/>
+      <c r="G7" s="295"/>
     </row>
     <row r="8" spans="1:7" s="86" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
@@ -6365,15 +6368,15 @@
       <c r="C8" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="290">
+      <c r="D8" s="294">
         <f>Page1!H5</f>
         <v>0</v>
       </c>
-      <c r="E8" s="290"/>
-      <c r="F8" s="272" t="s">
+      <c r="E8" s="294"/>
+      <c r="F8" s="276" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="275">
+      <c r="G8" s="279">
         <f>Page1!J5</f>
         <v>0</v>
       </c>
@@ -6386,15 +6389,15 @@
         <f>Page1!G44</f>
         <v>461309100</v>
       </c>
-      <c r="C9" s="272" t="s">
+      <c r="C9" s="276" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="278" t="s">
+      <c r="D9" s="282" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="279"/>
-      <c r="F9" s="273"/>
-      <c r="G9" s="276"/>
+      <c r="E9" s="283"/>
+      <c r="F9" s="277"/>
+      <c r="G9" s="280"/>
     </row>
     <row r="10" spans="1:7" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="97" t="s">
@@ -6404,34 +6407,34 @@
         <f>Page1!C5</f>
         <v>0</v>
       </c>
-      <c r="C10" s="274"/>
-      <c r="D10" s="280"/>
-      <c r="E10" s="281"/>
-      <c r="F10" s="274"/>
-      <c r="G10" s="277"/>
+      <c r="C10" s="278"/>
+      <c r="D10" s="284"/>
+      <c r="E10" s="285"/>
+      <c r="F10" s="278"/>
+      <c r="G10" s="281"/>
     </row>
     <row r="11" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="295" t="s">
+      <c r="A11" s="299" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="297" t="s">
+      <c r="B11" s="301" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="299" t="s">
+      <c r="C11" s="303" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="300"/>
-      <c r="E11" s="301"/>
-      <c r="F11" s="297" t="s">
+      <c r="D11" s="304"/>
+      <c r="E11" s="305"/>
+      <c r="F11" s="301" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="302" t="s">
+      <c r="G11" s="306" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="296"/>
-      <c r="B12" s="298"/>
+      <c r="A12" s="300"/>
+      <c r="B12" s="302"/>
       <c r="C12" s="99" t="s">
         <v>60</v>
       </c>
@@ -6441,8 +6444,8 @@
       <c r="E12" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="298"/>
-      <c r="G12" s="303"/>
+      <c r="F12" s="302"/>
+      <c r="G12" s="307"/>
     </row>
     <row r="13" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="100" t="s">
@@ -6512,7 +6515,7 @@
         <f>Page1!K39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="282" t="s">
+      <c r="G15" s="286" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6536,7 +6539,7 @@
         <f>Page2!F41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G16" s="223"/>
+      <c r="G16" s="227"/>
     </row>
     <row r="17" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="104" t="s">
@@ -6558,7 +6561,7 @@
         <f>Page1!I39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="223"/>
+      <c r="G17" s="227"/>
     </row>
     <row r="18" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="104" t="s">
@@ -6580,7 +6583,7 @@
         <f>Page2!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="223"/>
+      <c r="G18" s="227"/>
     </row>
     <row r="19" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="104" t="s">
@@ -6602,7 +6605,7 @@
         <f>Page1!J39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="223"/>
+      <c r="G19" s="227"/>
     </row>
     <row r="20" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="104" t="s">
@@ -6624,7 +6627,7 @@
         <f>Page2!E41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="223"/>
+      <c r="G20" s="227"/>
     </row>
     <row r="21" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="104" t="s">
@@ -6646,7 +6649,7 @@
         <f>Page1!G39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="223"/>
+      <c r="G21" s="227"/>
     </row>
     <row r="22" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="104" t="s">
@@ -6710,7 +6713,7 @@
       </c>
       <c r="E24" s="39">
         <f>Page2!J10</f>
-        <v>213</v>
+        <v>253</v>
       </c>
       <c r="F24" s="39" t="e">
         <f>Page2!I41</f>
@@ -6768,26 +6771,26 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="266" t="s">
+      <c r="A27" s="270" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="267"/>
-      <c r="C27" s="267"/>
-      <c r="D27" s="267"/>
-      <c r="E27" s="267"/>
-      <c r="F27" s="267"/>
-      <c r="G27" s="268"/>
+      <c r="B27" s="271"/>
+      <c r="C27" s="271"/>
+      <c r="D27" s="271"/>
+      <c r="E27" s="271"/>
+      <c r="F27" s="271"/>
+      <c r="G27" s="272"/>
     </row>
     <row r="28" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="250" t="s">
+      <c r="A28" s="254" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="251"/>
-      <c r="C28" s="269" t="s">
+      <c r="B28" s="255"/>
+      <c r="C28" s="273" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="270"/>
-      <c r="E28" s="271"/>
+      <c r="D28" s="274"/>
+      <c r="E28" s="275"/>
       <c r="F28" s="113" t="s">
         <v>92</v>
       </c>
@@ -6796,15 +6799,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="255" t="s">
+      <c r="A29" s="259" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="254"/>
-      <c r="C29" s="260" t="s">
+      <c r="B29" s="258"/>
+      <c r="C29" s="264" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="261"/>
-      <c r="E29" s="262"/>
+      <c r="D29" s="265"/>
+      <c r="E29" s="266"/>
       <c r="F29" s="66" t="s">
         <v>92</v>
       </c>
@@ -6813,15 +6816,15 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="255" t="s">
+      <c r="A30" s="259" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="254"/>
-      <c r="C30" s="260" t="s">
+      <c r="B30" s="258"/>
+      <c r="C30" s="264" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="261"/>
-      <c r="E30" s="262"/>
+      <c r="D30" s="265"/>
+      <c r="E30" s="266"/>
       <c r="F30" s="66" t="s">
         <v>92</v>
       </c>
@@ -6830,15 +6833,15 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="255" t="s">
+      <c r="A31" s="259" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="254"/>
-      <c r="C31" s="260" t="s">
+      <c r="B31" s="258"/>
+      <c r="C31" s="264" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="261"/>
-      <c r="E31" s="262"/>
+      <c r="D31" s="265"/>
+      <c r="E31" s="266"/>
       <c r="F31" s="66" t="s">
         <v>92</v>
       </c>
@@ -6847,15 +6850,15 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="255" t="s">
+      <c r="A32" s="259" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="254"/>
-      <c r="C32" s="260" t="s">
+      <c r="B32" s="258"/>
+      <c r="C32" s="264" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="261"/>
-      <c r="E32" s="262"/>
+      <c r="D32" s="265"/>
+      <c r="E32" s="266"/>
       <c r="F32" s="66" t="s">
         <v>92</v>
       </c>
@@ -6864,15 +6867,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="255" t="s">
+      <c r="A33" s="259" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="254"/>
-      <c r="C33" s="260" t="s">
+      <c r="B33" s="258"/>
+      <c r="C33" s="264" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="261"/>
-      <c r="E33" s="262"/>
+      <c r="D33" s="265"/>
+      <c r="E33" s="266"/>
       <c r="F33" s="66" t="s">
         <v>92</v>
       </c>
@@ -6885,11 +6888,11 @@
         <v>105</v>
       </c>
       <c r="B34" s="148"/>
-      <c r="C34" s="263" t="s">
+      <c r="C34" s="267" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="264"/>
-      <c r="E34" s="265"/>
+      <c r="D34" s="268"/>
+      <c r="E34" s="269"/>
       <c r="F34" s="114" t="s">
         <v>92</v>
       </c>
@@ -6898,25 +6901,25 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="266" t="s">
+      <c r="A35" s="270" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="267"/>
-      <c r="C35" s="267"/>
-      <c r="D35" s="267"/>
-      <c r="E35" s="267"/>
-      <c r="F35" s="267"/>
-      <c r="G35" s="268"/>
+      <c r="B35" s="271"/>
+      <c r="C35" s="271"/>
+      <c r="D35" s="271"/>
+      <c r="E35" s="271"/>
+      <c r="F35" s="271"/>
+      <c r="G35" s="272"/>
     </row>
     <row r="36" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="143" t="s">
         <v>108</v>
       </c>
       <c r="B36" s="144"/>
-      <c r="C36" s="258" t="s">
+      <c r="C36" s="262" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="259"/>
+      <c r="D36" s="263"/>
       <c r="E36" s="144"/>
       <c r="F36" s="10" t="s">
         <v>92</v>
@@ -6926,15 +6929,15 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="250" t="s">
+      <c r="A37" s="254" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="251"/>
-      <c r="C37" s="252" t="s">
+      <c r="B37" s="255"/>
+      <c r="C37" s="256" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="253"/>
-      <c r="E37" s="254"/>
+      <c r="D37" s="257"/>
+      <c r="E37" s="258"/>
       <c r="F37" s="106" t="s">
         <v>92</v>
       </c>
@@ -6943,15 +6946,15 @@
       </c>
     </row>
     <row r="38" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="255" t="s">
+      <c r="A38" s="259" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="254"/>
-      <c r="C38" s="252" t="s">
+      <c r="B38" s="258"/>
+      <c r="C38" s="256" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="253"/>
-      <c r="E38" s="254"/>
+      <c r="D38" s="257"/>
+      <c r="E38" s="258"/>
       <c r="F38" s="106" t="s">
         <v>92</v>
       </c>
@@ -6964,10 +6967,10 @@
         <v>113</v>
       </c>
       <c r="B39" s="148"/>
-      <c r="C39" s="256" t="s">
+      <c r="C39" s="260" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="257"/>
+      <c r="D39" s="261"/>
       <c r="E39" s="148"/>
       <c r="F39" s="1" t="s">
         <v>92</v>
@@ -6977,50 +6980,50 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="236" t="s">
+      <c r="A40" s="240" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="237"/>
-      <c r="C40" s="238" t="s">
+      <c r="B40" s="241"/>
+      <c r="C40" s="242" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="239"/>
-      <c r="E40" s="240"/>
-      <c r="F40" s="238" t="s">
+      <c r="D40" s="243"/>
+      <c r="E40" s="244"/>
+      <c r="F40" s="242" t="s">
         <v>138</v>
       </c>
-      <c r="G40" s="240"/>
+      <c r="G40" s="244"/>
     </row>
     <row r="41" spans="1:7" s="86" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="241"/>
-      <c r="B41" s="242"/>
-      <c r="C41" s="194"/>
-      <c r="D41" s="195"/>
-      <c r="E41" s="200"/>
-      <c r="F41" s="245"/>
-      <c r="G41" s="246"/>
+      <c r="A41" s="245"/>
+      <c r="B41" s="246"/>
+      <c r="C41" s="198"/>
+      <c r="D41" s="199"/>
+      <c r="E41" s="204"/>
+      <c r="F41" s="249"/>
+      <c r="G41" s="250"/>
     </row>
     <row r="42" spans="1:7" s="86" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="243"/>
-      <c r="B42" s="244"/>
-      <c r="C42" s="247" t="s">
+      <c r="A42" s="247"/>
+      <c r="B42" s="248"/>
+      <c r="C42" s="251" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="248"/>
-      <c r="E42" s="249"/>
-      <c r="F42" s="247" t="s">
+      <c r="D42" s="252"/>
+      <c r="E42" s="253"/>
+      <c r="F42" s="251" t="s">
         <v>139</v>
       </c>
-      <c r="G42" s="249"/>
+      <c r="G42" s="253"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="115"/>
       <c r="B43" s="115"/>
       <c r="C43" s="115"/>
       <c r="D43" s="115"/>
-      <c r="E43" s="234"/>
-      <c r="F43" s="234"/>
-      <c r="G43" s="234"/>
+      <c r="E43" s="238"/>
+      <c r="F43" s="238"/>
+      <c r="G43" s="238"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
@@ -7029,21 +7032,21 @@
       <c r="B44" s="116"/>
       <c r="C44" s="118"/>
       <c r="D44" s="115"/>
-      <c r="E44" s="235"/>
-      <c r="F44" s="235"/>
-      <c r="G44" s="235"/>
+      <c r="E44" s="239"/>
+      <c r="F44" s="239"/>
+      <c r="G44" s="239"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="283" t="s">
+      <c r="A46" s="287" t="s">
         <v>117</v>
       </c>
-      <c r="B46" s="283"/>
+      <c r="B46" s="287"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="283" t="s">
+      <c r="A47" s="287" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="283"/>
+      <c r="B47" s="287"/>
     </row>
   </sheetData>
   <mergeCells count="55">

</xml_diff>